<commit_message>
updated Bjt and footprints
</commit_message>
<xml_diff>
--- a/Kicad/Parts to order/Parts for senior design.xlsx
+++ b/Kicad/Parts to order/Parts for senior design.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cooki\Desktop\Classes\Senior design\Github\desg-of-senio\Kicad\Parts to order\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89CEA4F-118C-4106-84FD-72662EA70B2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23AF5DEE-9E86-4BDA-8927-109C82AAB839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21300" yWindow="2130" windowWidth="7500" windowHeight="6000" xr2:uid="{D75D6D5D-2919-4678-A5FB-CB7FB06746BB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D75D6D5D-2919-4678-A5FB-CB7FB06746BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t xml:space="preserve">Part </t>
   </si>
@@ -152,6 +151,9 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/espressif-systems/ESP32-WROOM-32D-4MB-HIGH-TEMP/12342929</t>
+  </si>
+  <si>
+    <t>led</t>
   </si>
 </sst>
 </file>
@@ -514,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{595E1ECF-B6D5-4FFC-B122-E1A98A24E039}">
-  <dimension ref="A1:P18"/>
+  <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,6 +784,11 @@
       </c>
       <c r="D18" s="1" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -808,6 +815,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009339DEEB0713054CA35A19C82B89FC7B" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bbdc801366e925ee4f0a09394e11d53f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="501d98d0-dd6a-4103-a181-3e0b7e01b984" xmlns:ns4="c0f1a386-a454-4bbc-ac7b-d0261faf4843" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2092042c42a9a998b551227d8bb769db" ns3:_="" ns4:_="">
     <xsd:import namespace="501d98d0-dd6a-4103-a181-3e0b7e01b984"/>
@@ -1016,15 +1032,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1032,6 +1039,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF0A9CA0-081D-4246-8241-4C60799D2700}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD0B4D4D-2C28-451D-AE19-A64DD69378C1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1046,14 +1061,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF0A9CA0-081D-4246-8241-4C60799D2700}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Update Parts for senior design.xlsx
</commit_message>
<xml_diff>
--- a/Kicad/Parts to order/Parts for senior design.xlsx
+++ b/Kicad/Parts to order/Parts for senior design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cooki\Desktop\Classes\Senior design\Github\desg-of-senio\Kicad\Parts to order\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23AF5DEE-9E86-4BDA-8927-109C82AAB839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05CDC16C-2A63-483A-89FF-A442E60DB5FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D75D6D5D-2919-4678-A5FB-CB7FB06746BB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t xml:space="preserve">Part </t>
   </si>
@@ -153,7 +153,10 @@
     <t>https://www.digikey.com/en/products/detail/espressif-systems/ESP32-WROOM-32D-4MB-HIGH-TEMP/12342929</t>
   </si>
   <si>
-    <t>led</t>
+    <t>relay</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/sanyou-relay/SRD-S-112DM-F-11/14548486</t>
   </si>
 </sst>
 </file>
@@ -519,7 +522,7 @@
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,6 +792,15 @@
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>39</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>2.98</v>
+      </c>
+      <c r="D19" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -815,15 +827,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009339DEEB0713054CA35A19C82B89FC7B" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bbdc801366e925ee4f0a09394e11d53f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="501d98d0-dd6a-4103-a181-3e0b7e01b984" xmlns:ns4="c0f1a386-a454-4bbc-ac7b-d0261faf4843" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2092042c42a9a998b551227d8bb769db" ns3:_="" ns4:_="">
     <xsd:import namespace="501d98d0-dd6a-4103-a181-3e0b7e01b984"/>
@@ -1032,6 +1035,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1039,14 +1051,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF0A9CA0-081D-4246-8241-4C60799D2700}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD0B4D4D-2C28-451D-AE19-A64DD69378C1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1061,6 +1065,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF0A9CA0-081D-4246-8241-4C60799D2700}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
added footprint list to excel and added power supply footprint
</commit_message>
<xml_diff>
--- a/Kicad/Parts to order/Parts for senior design.xlsx
+++ b/Kicad/Parts to order/Parts for senior design.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cooki\Desktop\Classes\Senior design\Github\desg-of-senio\Kicad\Parts to order\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\massj\Documents\desg-of-senio\Kicad\Parts to order\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05CDC16C-2A63-483A-89FF-A442E60DB5FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C1B1BE-B1B7-4C02-943E-2D0C7B3D55C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D75D6D5D-2919-4678-A5FB-CB7FB06746BB}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{D75D6D5D-2919-4678-A5FB-CB7FB06746BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t xml:space="preserve">Part </t>
   </si>
@@ -157,13 +157,49 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/sanyou-relay/SRD-S-112DM-F-11/14548486</t>
+  </si>
+  <si>
+    <t>foot</t>
+  </si>
+  <si>
+    <t>2917 (7343 Metric)</t>
+  </si>
+  <si>
+    <t>1411 (3528 Metric)</t>
+  </si>
+  <si>
+    <t>0402 (1005 Metric)</t>
+  </si>
+  <si>
+    <t>1206 (3216 Metric)</t>
+  </si>
+  <si>
+    <t>TO-252-3, DPak (2 Leads + Tab), SC-63</t>
+  </si>
+  <si>
+    <t>28-VFQFN Exposed Pad</t>
+  </si>
+  <si>
+    <t>DO-214AC, SMA</t>
+  </si>
+  <si>
+    <t>0805 (2012 Metric)</t>
+  </si>
+  <si>
+    <t>1210 (3225 Metric)</t>
+  </si>
+  <si>
+    <t>SC-90, SOD-323F</t>
+  </si>
+  <si>
+    <t>TO-261-4, TO-261AA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,6 +214,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF444444"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="2">
@@ -201,9 +242,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -522,16 +564,17 @@
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -544,8 +587,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -558,8 +604,11 @@
       <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F2" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -572,8 +621,11 @@
       <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F3" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -586,8 +638,11 @@
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F4" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -600,8 +655,11 @@
       <c r="D5" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F5" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -614,6 +672,9 @@
       <c r="D6" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="F6" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="N6" t="s">
         <v>14</v>
       </c>
@@ -621,7 +682,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -634,8 +695,11 @@
       <c r="D7" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F7" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -649,7 +713,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -662,8 +726,11 @@
       <c r="D9" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F9" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -677,7 +744,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -687,11 +754,14 @@
       <c r="C11">
         <v>0.1</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F11" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -704,8 +774,11 @@
       <c r="D12" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F12" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -718,8 +791,11 @@
       <c r="D13" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F13" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -732,8 +808,11 @@
       <c r="D14" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F14" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -746,8 +825,11 @@
       <c r="D15" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F15" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -760,8 +842,11 @@
       <c r="D16" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F16" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -774,8 +859,11 @@
       <c r="D17" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F17" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -789,7 +877,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -820,13 +908,23 @@
     <hyperlink ref="D16" r:id="rId13" xr:uid="{B73E2357-2267-4543-A874-D84EA92CB61E}"/>
     <hyperlink ref="D17" r:id="rId14" xr:uid="{DFAE2C83-32D2-4CDF-A31C-96683BC27714}"/>
     <hyperlink ref="D18" r:id="rId15" xr:uid="{FDE28B73-190C-4453-B1AE-EB4B2D48AC4E}"/>
+    <hyperlink ref="D11" r:id="rId16" xr:uid="{8623EF09-1ACD-460F-B9A7-87C01066BD5B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId16"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId17"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009339DEEB0713054CA35A19C82B89FC7B" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bbdc801366e925ee4f0a09394e11d53f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="501d98d0-dd6a-4103-a181-3e0b7e01b984" xmlns:ns4="c0f1a386-a454-4bbc-ac7b-d0261faf4843" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2092042c42a9a998b551227d8bb769db" ns3:_="" ns4:_="">
     <xsd:import namespace="501d98d0-dd6a-4103-a181-3e0b7e01b984"/>
@@ -1035,15 +1133,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1051,6 +1140,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF0A9CA0-081D-4246-8241-4C60799D2700}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD0B4D4D-2C28-451D-AE19-A64DD69378C1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1065,14 +1162,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF0A9CA0-081D-4246-8241-4C60799D2700}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>